<commit_message>
Completed First Half of Loop
</commit_message>
<xml_diff>
--- a/Callibration/Sensor Callibrations.xlsx
+++ b/Callibration/Sensor Callibrations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielchvat/Desktop/ECE 3 Robot/Callibration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8205C5E-D92F-824B-9F05-939C971D7BE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC8F8696-C9F7-E74E-A21A-8CAEDCA97518}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16340" activeTab="3" xr2:uid="{2364EECD-9656-9943-8B8F-8172E039B3CE}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16200" activeTab="3" xr2:uid="{2364EECD-9656-9943-8B8F-8172E039B3CE}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw" sheetId="1" r:id="rId1"/>
@@ -18,15 +18,7 @@
     <sheet name="Normalized" sheetId="3" r:id="rId3"/>
     <sheet name="Sensor Fusion" sheetId="4" r:id="rId4"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'Sensor Fusion'!$K$1</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'Sensor Fusion'!$K$2:$K$26</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'Sensor Fusion'!$L$1</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'Sensor Fusion'!$L$2:$L$26</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'Sensor Fusion'!$M$1</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">'Sensor Fusion'!$M$2:$M$26</definedName>
-  </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -47,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="19">
   <si>
     <t>ERROR</t>
   </si>
@@ -92,6 +84,18 @@
   </si>
   <si>
     <t>(15-14-12-10) / 8</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>Base Speed</t>
+  </si>
+  <si>
+    <t>Kp</t>
   </si>
 </sst>
 </file>
@@ -3574,10 +3578,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Sensor Fusion'!$K$2:$K$26</c:f>
+              <c:f>'Sensor Fusion'!$K$2:$K$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>-40</c:v>
                 </c:pt>
@@ -3646,10 +3650,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Sensor Fusion'!$L$2:$L$26</c:f>
+              <c:f>'Sensor Fusion'!$L$2:$L$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>-1403.3526655750002</c:v>
                 </c:pt>
@@ -3763,10 +3767,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Sensor Fusion'!$K$2:$K$26</c:f>
+              <c:f>'Sensor Fusion'!$K$2:$K$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>-40</c:v>
                 </c:pt>
@@ -3835,10 +3839,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Sensor Fusion'!$M$2:$M$26</c:f>
+              <c:f>'Sensor Fusion'!$M$2:$M$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>-1315.7500216750002</c:v>
                 </c:pt>
@@ -5877,16 +5881,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>127000</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>768350</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8639,10 +8643,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E14E31A0-E81F-7844-B93B-57918A88D870}">
-  <dimension ref="A1:M26"/>
+  <dimension ref="A1:O50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O29" sqref="O29"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8650,7 +8654,7 @@
     <col min="12" max="12" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -8687,8 +8691,11 @@
       <c r="M1" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>-40</v>
       </c>
@@ -8724,11 +8731,14 @@
         <v>-1403.3526655750002</v>
       </c>
       <c r="M2">
-        <f xml:space="preserve"> (-10 * $E2 + 10 * $F2 + -12* $D2 + 12 *$G2 + -14 * $C2 + 14 * $H2 + -15 * $B2 +15 * $I2)/8</f>
+        <f xml:space="preserve"> (-10 * $E2 + 10 * $F2 + -12* $D2 + 12 *$G2 + -14 * $C2 + 14 * $H2 + -15 * $B2 +15 * $I2)/8 * $O$2</f>
         <v>-1315.7500216750002</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>-36</v>
       </c>
@@ -8764,11 +8774,11 @@
         <v>-2088.6849499999998</v>
       </c>
       <c r="M3">
-        <f t="shared" ref="M3:M22" si="1" xml:space="preserve"> (-10 * $E3 + 10 * $F3 + -12* $D3 + 12 *$G3 + -14 * $C3 + 14 * $H3 + -15 * $B3 +15 * $I3)/8</f>
+        <f t="shared" ref="M3:M22" si="1" xml:space="preserve"> (-10 * $E3 + 10 * $F3 + -12* $D3 + 12 *$G3 + -14 * $C3 + 14 * $H3 + -15 * $B3 +15 * $I3)/8 * $O$2</f>
         <v>-2034.6082259375</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>-32</v>
       </c>
@@ -8808,7 +8818,7 @@
         <v>-1750.7157924849998</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>-28</v>
       </c>
@@ -8848,7 +8858,7 @@
         <v>-2040.6725410499998</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>-24</v>
       </c>
@@ -8888,7 +8898,7 @@
         <v>-1694.9622791250001</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>-20</v>
       </c>
@@ -8928,7 +8938,7 @@
         <v>-1430.0827891249999</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>-16</v>
       </c>
@@ -8968,7 +8978,7 @@
         <v>-1643.6416280499998</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>-12</v>
       </c>
@@ -9008,7 +9018,7 @@
         <v>-1129.5359951249998</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>-8</v>
       </c>
@@ -9048,7 +9058,7 @@
         <v>-1373.9618246499999</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>-4</v>
       </c>
@@ -9088,7 +9098,7 @@
         <v>-1085.7559524687499</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>0</v>
       </c>
@@ -9128,7 +9138,7 @@
         <v>256.20170501250004</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>4</v>
       </c>
@@ -9168,7 +9178,7 @@
         <v>1305.6504132800001</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>8</v>
       </c>
@@ -9208,7 +9218,7 @@
         <v>1007.3727729125</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>12</v>
       </c>
@@ -9248,7 +9258,7 @@
         <v>1615.6526399875002</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>16</v>
       </c>
@@ -9537,16 +9547,336 @@
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
+      <c r="K23" t="s">
+        <v>15</v>
+      </c>
+      <c r="L23">
+        <f>MIN(L2:L22)</f>
+        <v>-2088.6849499999998</v>
+      </c>
+      <c r="M23">
+        <f>MIN(M2:M22)</f>
+        <v>-2040.6725410499998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K24" t="s">
+        <v>16</v>
+      </c>
+      <c r="L24">
+        <f>MAX(L2:L22)</f>
+        <v>2049.3612767750001</v>
+      </c>
+      <c r="M24">
+        <f>MAX(M2:M22)</f>
+        <v>2119.9683037499999</v>
+      </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>12</v>
       </c>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>13</v>
       </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="J27" t="s">
+        <v>17</v>
+      </c>
+      <c r="K27" t="s">
+        <v>0</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="J28">
+        <v>20</v>
+      </c>
+      <c r="K28">
+        <v>-40</v>
+      </c>
+      <c r="L28">
+        <f xml:space="preserve"> (2 * ((L2 -$L$23) / ($L$24 -$L$23)) - 1) * (255 - $J$28)</f>
+        <v>-157.15984161907627</v>
+      </c>
+      <c r="M28">
+        <f xml:space="preserve"> (2 * ((M2 -$M$23) / ($M$24 -$M$23)) - 1) * (255 - $J$28)</f>
+        <v>-153.11031117187724</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K29">
+        <v>-36</v>
+      </c>
+      <c r="L29">
+        <f t="shared" ref="L29:L48" si="2" xml:space="preserve"> (2 * ((L3 -$L$23) / ($L$24 -$L$23)) - 1) * (255 - $J$28)</f>
+        <v>-235</v>
+      </c>
+      <c r="M29">
+        <f t="shared" ref="M29:M48" si="3" xml:space="preserve"> (2 * ((M3 -$M$23) / ($M$24 -$M$23)) - 1) * (255 - $J$28)</f>
+        <v>-234.31495454445746</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K30">
+        <v>-32</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="2"/>
+        <v>-177.38658010711657</v>
+      </c>
+      <c r="M30">
+        <f t="shared" si="3"/>
+        <v>-202.24550930756897</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K31">
+        <v>-28</v>
+      </c>
+      <c r="L31">
+        <f t="shared" si="2"/>
+        <v>-145.0373652338632</v>
+      </c>
+      <c r="M31">
+        <f t="shared" si="3"/>
+        <v>-235</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K32">
+        <v>-24</v>
+      </c>
+      <c r="L32">
+        <f t="shared" si="2"/>
+        <v>-99.748058078017777</v>
+      </c>
+      <c r="M32">
+        <f t="shared" si="3"/>
+        <v>-195.9474046990085</v>
+      </c>
+    </row>
+    <row r="33" spans="11:13" x14ac:dyDescent="0.2">
+      <c r="K33">
+        <v>-20</v>
+      </c>
+      <c r="L33">
+        <f t="shared" si="2"/>
+        <v>-65.400349319633193</v>
+      </c>
+      <c r="M33">
+        <f t="shared" si="3"/>
+        <v>-166.02572557700668</v>
+      </c>
+    </row>
+    <row r="34" spans="11:13" x14ac:dyDescent="0.2">
+      <c r="K34">
+        <v>-16</v>
+      </c>
+      <c r="L34">
+        <f t="shared" si="2"/>
+        <v>-60.969816904148686</v>
+      </c>
+      <c r="M34">
+        <f t="shared" si="3"/>
+        <v>-190.15005114098716</v>
+      </c>
+    </row>
+    <row r="35" spans="11:13" x14ac:dyDescent="0.2">
+      <c r="K35">
+        <v>-12</v>
+      </c>
+      <c r="L35">
+        <f t="shared" si="2"/>
+        <v>-36.44413228485304</v>
+      </c>
+      <c r="M35">
+        <f t="shared" si="3"/>
+        <v>-132.0749476922623</v>
+      </c>
+    </row>
+    <row r="36" spans="11:13" x14ac:dyDescent="0.2">
+      <c r="K36">
+        <v>-8</v>
+      </c>
+      <c r="L36">
+        <f t="shared" si="2"/>
+        <v>-34.157413172866548</v>
+      </c>
+      <c r="M36">
+        <f t="shared" si="3"/>
+        <v>-159.68611245317362</v>
+      </c>
+    </row>
+    <row r="37" spans="11:13" x14ac:dyDescent="0.2">
+      <c r="K37">
+        <v>-4</v>
+      </c>
+      <c r="L37">
+        <f t="shared" si="2"/>
+        <v>-20.664416996899455</v>
+      </c>
+      <c r="M37">
+        <f t="shared" si="3"/>
+        <v>-127.12940665279616</v>
+      </c>
+    </row>
+    <row r="38" spans="11:13" x14ac:dyDescent="0.2">
+      <c r="K38">
+        <v>0</v>
+      </c>
+      <c r="L38">
+        <f t="shared" si="2"/>
+        <v>8.2092200505333075</v>
+      </c>
+      <c r="M38">
+        <f t="shared" si="3"/>
+        <v>24.462649124973275</v>
+      </c>
+    </row>
+    <row r="39" spans="11:13" x14ac:dyDescent="0.2">
+      <c r="K39">
+        <v>4</v>
+      </c>
+      <c r="L39">
+        <f t="shared" si="2"/>
+        <v>34.209168957773947</v>
+      </c>
+      <c r="M39">
+        <f t="shared" si="3"/>
+        <v>143.0119090309758</v>
+      </c>
+    </row>
+    <row r="40" spans="11:13" x14ac:dyDescent="0.2">
+      <c r="K40">
+        <v>8</v>
+      </c>
+      <c r="L40">
+        <f t="shared" si="2"/>
+        <v>31.196592553289104</v>
+      </c>
+      <c r="M40">
+        <f t="shared" si="3"/>
+        <v>109.31746238150444</v>
+      </c>
+    </row>
+    <row r="41" spans="11:13" x14ac:dyDescent="0.2">
+      <c r="K41">
+        <v>12</v>
+      </c>
+      <c r="L41">
+        <f t="shared" si="2"/>
+        <v>62.136676546026791</v>
+      </c>
+      <c r="M41">
+        <f t="shared" si="3"/>
+        <v>178.03080443374131</v>
+      </c>
+    </row>
+    <row r="42" spans="11:13" x14ac:dyDescent="0.2">
+      <c r="K42">
+        <v>16</v>
+      </c>
+      <c r="L42">
+        <f t="shared" si="2"/>
+        <v>77.473034607880763</v>
+      </c>
+      <c r="M42">
+        <f t="shared" si="3"/>
+        <v>195.26987936309214</v>
+      </c>
+    </row>
+    <row r="43" spans="11:13" x14ac:dyDescent="0.2">
+      <c r="K43">
+        <v>20</v>
+      </c>
+      <c r="L43">
+        <f t="shared" si="2"/>
+        <v>75.294887624286162</v>
+      </c>
+      <c r="M43">
+        <f t="shared" si="3"/>
+        <v>148.7441566797863</v>
+      </c>
+    </row>
+    <row r="44" spans="11:13" x14ac:dyDescent="0.2">
+      <c r="K44">
+        <v>24</v>
+      </c>
+      <c r="L44">
+        <f t="shared" si="2"/>
+        <v>132.42846351198372</v>
+      </c>
+      <c r="M44">
+        <f t="shared" si="3"/>
+        <v>216.11811586037018</v>
+      </c>
+    </row>
+    <row r="45" spans="11:13" x14ac:dyDescent="0.2">
+      <c r="K45">
+        <v>28</v>
+      </c>
+      <c r="L45">
+        <f t="shared" si="2"/>
+        <v>153.0422947703961</v>
+      </c>
+      <c r="M45">
+        <f t="shared" si="3"/>
+        <v>200.85107722688329</v>
+      </c>
+    </row>
+    <row r="46" spans="11:13" x14ac:dyDescent="0.2">
+      <c r="K46">
+        <v>32</v>
+      </c>
+      <c r="L46">
+        <f t="shared" si="2"/>
+        <v>235</v>
+      </c>
+      <c r="M46">
+        <f t="shared" si="3"/>
+        <v>235</v>
+      </c>
+    </row>
+    <row r="47" spans="11:13" x14ac:dyDescent="0.2">
+      <c r="K47">
+        <v>36</v>
+      </c>
+      <c r="L47">
+        <f t="shared" si="2"/>
+        <v>231.18968619592047</v>
+      </c>
+      <c r="M47">
+        <f t="shared" si="3"/>
+        <v>211.7380614511525</v>
+      </c>
+    </row>
+    <row r="48" spans="11:13" x14ac:dyDescent="0.2">
+      <c r="K48">
+        <v>40</v>
+      </c>
+      <c r="L48">
+        <f t="shared" si="2"/>
+        <v>63.76858043040243</v>
+      </c>
+      <c r="M48">
+        <f t="shared" si="3"/>
+        <v>52.832676635479672</v>
+      </c>
+    </row>
+    <row r="50" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L50" s="1"/>
+      <c r="M50" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>